<commit_message>
Build Before And After Comparison
Create "Before And After Comparison" Front end and Back end. Some Validation needed but code is running when expected input is provided.
</commit_message>
<xml_diff>
--- a/DataFolder/River_1-24_O/SlopeSheet.xlsx
+++ b/DataFolder/River_1-24_O/SlopeSheet.xlsx
@@ -15,9 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>KTC Topography Report Lanes  23 - 24</t>
+    <t>KTC Topography Report</t>
+  </si>
+  <si>
+    <t>Lane  12</t>
   </si>
 </sst>
 </file>
@@ -79,10 +82,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>565150</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -101,7 +104,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="323850"/>
-          <a:ext cx="6350000" cy="10795000"/>
+          <a:ext cx="5715000" cy="13970000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -113,16 +116,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -140,8 +143,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5175250" y="323850"/>
-          <a:ext cx="6350000" cy="10795000"/>
+          <a:off x="5105400" y="323850"/>
+          <a:ext cx="5715000" cy="13970000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -153,13 +156,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>215900</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>73025</xdr:rowOff>
@@ -180,88 +183,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4565650" y="1619250"/>
+          <a:off x="4495800" y="1619250"/>
           <a:ext cx="825500" cy="4445000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>488950</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>111125</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1028" name="Picture 4"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="11334750"/>
-          <a:ext cx="4445000" cy="2540000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>177800</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>111125</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1029" name="Picture 5"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="5175250" y="11334750"/>
-          <a:ext cx="4445000" cy="2540000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -574,7 +497,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="K1:K1"/>
+  <dimension ref="J1:R2"/>
   <sheetViews>
     <sheetView defaultGridColor="0" colorId="64" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -586,85 +509,32 @@
     <col min="3" max="4" width="6.666667" customWidth="1"/>
     <col min="5" max="5" width="5.238095" customWidth="1"/>
     <col min="6" max="8" width="0" customWidth="1"/>
-    <col min="9" max="10" width="6.666667" customWidth="1"/>
+    <col min="9" max="9" width="14.7619" customWidth="1"/>
+    <col min="10" max="10" width="6.666667" customWidth="1"/>
+    <col min="17" max="17" width="14.28571" customWidth="1"/>
     <col min="30" max="30" width="3.809524" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="11:11">
-      <c r="K1" s="1" t="s">
+    <row r="1" spans="14:14">
+      <c r="N1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="11:11"/>
-    <row r="3" spans="11:11"/>
-    <row r="4" spans="11:11"/>
-    <row r="5" spans="11:11"/>
-    <row r="6" spans="11:11"/>
-    <row r="7" spans="11:11"/>
-    <row r="8" spans="11:11"/>
-    <row r="9" spans="11:11"/>
-    <row r="10" spans="11:11"/>
-    <row r="11" spans="11:11"/>
-    <row r="12" spans="11:11"/>
-    <row r="13" spans="11:11"/>
-    <row r="14" spans="11:11"/>
-    <row r="15" spans="11:11"/>
-    <row r="16" spans="11:11"/>
-    <row r="17" spans="11:11"/>
-    <row r="18" spans="11:11"/>
-    <row r="19" spans="11:11"/>
-    <row r="20" spans="11:11"/>
-    <row r="21" spans="11:11"/>
-    <row r="22" spans="11:11"/>
-    <row r="23" spans="11:11"/>
-    <row r="24" spans="11:11"/>
-    <row r="25" spans="11:11"/>
-    <row r="26" spans="11:11"/>
-    <row r="27" spans="11:11"/>
-    <row r="28" spans="11:11"/>
-    <row r="29" spans="11:11"/>
-    <row r="30" spans="11:11"/>
-    <row r="31" spans="11:11"/>
-    <row r="32" spans="11:11"/>
-    <row r="33" spans="11:11"/>
-    <row r="34" spans="11:11"/>
-    <row r="35" spans="11:11"/>
-    <row r="36" spans="11:11"/>
-    <row r="37" spans="11:11"/>
-    <row r="38" spans="11:11"/>
-    <row r="39" spans="11:11"/>
-    <row r="40" spans="11:11"/>
-    <row r="41" spans="11:11"/>
-    <row r="42" spans="11:11"/>
-    <row r="43" spans="11:11"/>
-    <row r="44" spans="11:11"/>
-    <row r="45" spans="11:11"/>
-    <row r="46" spans="11:11"/>
-    <row r="47" spans="11:11"/>
-    <row r="48" spans="11:11"/>
-    <row r="49" spans="11:11"/>
-    <row r="50" spans="11:11"/>
-    <row r="51" spans="11:11"/>
-    <row r="52" spans="11:11"/>
-    <row r="53" spans="11:11"/>
-    <row r="54" spans="11:11"/>
-    <row r="55" spans="11:11"/>
-    <row r="56" spans="11:11"/>
-    <row r="57" spans="11:11"/>
-    <row r="58" spans="11:11"/>
-    <row r="59" spans="11:11"/>
-    <row r="60" spans="11:11"/>
-    <row r="61" spans="11:11"/>
-    <row r="62" spans="11:11"/>
-    <row r="63" spans="11:11"/>
-    <row r="64" spans="11:11"/>
-    <row r="65" spans="11:11"/>
-    <row r="66" spans="11:11"/>
-    <row r="67" spans="11:11"/>
-    <row r="68" spans="11:11"/>
-    <row r="69" spans="11:11"/>
-    <row r="70" spans="11:11"/>
-    <row r="71" spans="11:11"/>
+    <row r="2" spans="10:18">
+      <c r="J2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" s="1"/>
+    </row>
+    <row r="3" spans="10:18"/>
+    <row r="4" spans="10:18"/>
+    <row r="5" spans="10:18"/>
+    <row r="6" spans="10:18"/>
+    <row r="7" spans="10:18"/>
+    <row r="8" spans="10:18"/>
+    <row r="9" spans="10:18"/>
+    <row r="10" spans="10:18"/>
+    <row r="11" spans="10:18"/>
   </sheetData>
   <pageMargins left="1" right="0" top="0.25" bottom="0" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="70" orientation="portrait"/>

</xml_diff>

<commit_message>
Changed upload Format of XML in order to match the new LaneMapper.Exe
Makes change in the substring. Delete the part where the xml Upload to server with date and time attached the file name.

Also a new Version of Lane Mapper was deploy. This one create reports in a different format and have multi instances capabilities.
</commit_message>
<xml_diff>
--- a/DataFolder/River_1-24_O/SlopeSheet.xlsx
+++ b/DataFolder/River_1-24_O/SlopeSheet.xlsx
@@ -15,12 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>KTC Topography Report</t>
-  </si>
-  <si>
-    <t>Lane  12</t>
+    <t>KTC Topography Report Lanes  23 - 24</t>
   </si>
 </sst>
 </file>
@@ -82,10 +79,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>88</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>565150</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -104,7 +101,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="323850"/>
-          <a:ext cx="5715000" cy="13970000"/>
+          <a:ext cx="6350000" cy="10795000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -116,16 +113,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>88</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -143,8 +140,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5105400" y="323850"/>
-          <a:ext cx="5715000" cy="13970000"/>
+          <a:off x="5175250" y="323850"/>
+          <a:ext cx="6350000" cy="10795000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -156,13 +153,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>215900</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>73025</xdr:rowOff>
@@ -183,8 +180,88 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4495800" y="1619250"/>
+          <a:off x="4565650" y="1619250"/>
           <a:ext cx="825500" cy="4445000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>488950</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>111125</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1028" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="11334750"/>
+          <a:ext cx="4445000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>111125</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1029" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5175250" y="11334750"/>
+          <a:ext cx="4445000" cy="2540000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -497,7 +574,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="J1:R2"/>
+  <dimension ref="K1:K1"/>
   <sheetViews>
     <sheetView defaultGridColor="0" colorId="64" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -509,32 +586,85 @@
     <col min="3" max="4" width="6.666667" customWidth="1"/>
     <col min="5" max="5" width="5.238095" customWidth="1"/>
     <col min="6" max="8" width="0" customWidth="1"/>
-    <col min="9" max="9" width="14.7619" customWidth="1"/>
-    <col min="10" max="10" width="6.666667" customWidth="1"/>
-    <col min="17" max="17" width="14.28571" customWidth="1"/>
+    <col min="9" max="10" width="6.666667" customWidth="1"/>
     <col min="30" max="30" width="3.809524" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="14:14">
-      <c r="N1" s="1" t="s">
+    <row r="1" spans="11:11">
+      <c r="K1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="10:18">
-      <c r="J2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="R2" s="1"/>
-    </row>
-    <row r="3" spans="10:18"/>
-    <row r="4" spans="10:18"/>
-    <row r="5" spans="10:18"/>
-    <row r="6" spans="10:18"/>
-    <row r="7" spans="10:18"/>
-    <row r="8" spans="10:18"/>
-    <row r="9" spans="10:18"/>
-    <row r="10" spans="10:18"/>
-    <row r="11" spans="10:18"/>
+    <row r="2" spans="11:11"/>
+    <row r="3" spans="11:11"/>
+    <row r="4" spans="11:11"/>
+    <row r="5" spans="11:11"/>
+    <row r="6" spans="11:11"/>
+    <row r="7" spans="11:11"/>
+    <row r="8" spans="11:11"/>
+    <row r="9" spans="11:11"/>
+    <row r="10" spans="11:11"/>
+    <row r="11" spans="11:11"/>
+    <row r="12" spans="11:11"/>
+    <row r="13" spans="11:11"/>
+    <row r="14" spans="11:11"/>
+    <row r="15" spans="11:11"/>
+    <row r="16" spans="11:11"/>
+    <row r="17" spans="11:11"/>
+    <row r="18" spans="11:11"/>
+    <row r="19" spans="11:11"/>
+    <row r="20" spans="11:11"/>
+    <row r="21" spans="11:11"/>
+    <row r="22" spans="11:11"/>
+    <row r="23" spans="11:11"/>
+    <row r="24" spans="11:11"/>
+    <row r="25" spans="11:11"/>
+    <row r="26" spans="11:11"/>
+    <row r="27" spans="11:11"/>
+    <row r="28" spans="11:11"/>
+    <row r="29" spans="11:11"/>
+    <row r="30" spans="11:11"/>
+    <row r="31" spans="11:11"/>
+    <row r="32" spans="11:11"/>
+    <row r="33" spans="11:11"/>
+    <row r="34" spans="11:11"/>
+    <row r="35" spans="11:11"/>
+    <row r="36" spans="11:11"/>
+    <row r="37" spans="11:11"/>
+    <row r="38" spans="11:11"/>
+    <row r="39" spans="11:11"/>
+    <row r="40" spans="11:11"/>
+    <row r="41" spans="11:11"/>
+    <row r="42" spans="11:11"/>
+    <row r="43" spans="11:11"/>
+    <row r="44" spans="11:11"/>
+    <row r="45" spans="11:11"/>
+    <row r="46" spans="11:11"/>
+    <row r="47" spans="11:11"/>
+    <row r="48" spans="11:11"/>
+    <row r="49" spans="11:11"/>
+    <row r="50" spans="11:11"/>
+    <row r="51" spans="11:11"/>
+    <row r="52" spans="11:11"/>
+    <row r="53" spans="11:11"/>
+    <row r="54" spans="11:11"/>
+    <row r="55" spans="11:11"/>
+    <row r="56" spans="11:11"/>
+    <row r="57" spans="11:11"/>
+    <row r="58" spans="11:11"/>
+    <row r="59" spans="11:11"/>
+    <row r="60" spans="11:11"/>
+    <row r="61" spans="11:11"/>
+    <row r="62" spans="11:11"/>
+    <row r="63" spans="11:11"/>
+    <row r="64" spans="11:11"/>
+    <row r="65" spans="11:11"/>
+    <row r="66" spans="11:11"/>
+    <row r="67" spans="11:11"/>
+    <row r="68" spans="11:11"/>
+    <row r="69" spans="11:11"/>
+    <row r="70" spans="11:11"/>
+    <row r="71" spans="11:11"/>
   </sheetData>
   <pageMargins left="1" right="0" top="0.25" bottom="0" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="70" orientation="portrait"/>

</xml_diff>

<commit_message>
Fixed an issue with the processing Script that causes unwanted delete of files
</commit_message>
<xml_diff>
--- a/DataFolder/River_1-24_O/SlopeSheet.xlsx
+++ b/DataFolder/River_1-24_O/SlopeSheet.xlsx
@@ -15,9 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>ABC Bowling Center Lanes  23 - 24</t>
+    <t>ABC Bowling Center</t>
+  </si>
+  <si>
+    <t>Lane  12</t>
   </si>
 </sst>
 </file>
@@ -79,10 +82,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>565150</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -101,7 +104,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="323850"/>
-          <a:ext cx="6350000" cy="10795000"/>
+          <a:ext cx="5715000" cy="13970000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -113,16 +116,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -140,8 +143,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5175250" y="323850"/>
-          <a:ext cx="6350000" cy="10795000"/>
+          <a:off x="5105400" y="323850"/>
+          <a:ext cx="5715000" cy="13970000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -153,13 +156,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>215900</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>73025</xdr:rowOff>
@@ -180,88 +183,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4565650" y="1619250"/>
+          <a:off x="4495800" y="1619250"/>
           <a:ext cx="825500" cy="4445000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>488950</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>111125</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1028" name="Picture 4"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="11334750"/>
-          <a:ext cx="4445000" cy="2540000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>177800</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>111125</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1029" name="Picture 5"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="5175250" y="11334750"/>
-          <a:ext cx="4445000" cy="2540000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -574,7 +497,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="K1:K1"/>
+  <dimension ref="J1:R2"/>
   <sheetViews>
     <sheetView defaultGridColor="0" colorId="64" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -586,85 +509,32 @@
     <col min="3" max="4" width="6.666667" customWidth="1"/>
     <col min="5" max="5" width="5.238095" customWidth="1"/>
     <col min="6" max="8" width="0" customWidth="1"/>
-    <col min="9" max="10" width="6.666667" customWidth="1"/>
+    <col min="9" max="9" width="14.7619" customWidth="1"/>
+    <col min="10" max="10" width="6.666667" customWidth="1"/>
+    <col min="17" max="17" width="14.28571" customWidth="1"/>
     <col min="30" max="30" width="3.809524" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="11:11">
-      <c r="K1" s="1" t="s">
+    <row r="1" spans="14:14">
+      <c r="N1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="11:11"/>
-    <row r="3" spans="11:11"/>
-    <row r="4" spans="11:11"/>
-    <row r="5" spans="11:11"/>
-    <row r="6" spans="11:11"/>
-    <row r="7" spans="11:11"/>
-    <row r="8" spans="11:11"/>
-    <row r="9" spans="11:11"/>
-    <row r="10" spans="11:11"/>
-    <row r="11" spans="11:11"/>
-    <row r="12" spans="11:11"/>
-    <row r="13" spans="11:11"/>
-    <row r="14" spans="11:11"/>
-    <row r="15" spans="11:11"/>
-    <row r="16" spans="11:11"/>
-    <row r="17" spans="11:11"/>
-    <row r="18" spans="11:11"/>
-    <row r="19" spans="11:11"/>
-    <row r="20" spans="11:11"/>
-    <row r="21" spans="11:11"/>
-    <row r="22" spans="11:11"/>
-    <row r="23" spans="11:11"/>
-    <row r="24" spans="11:11"/>
-    <row r="25" spans="11:11"/>
-    <row r="26" spans="11:11"/>
-    <row r="27" spans="11:11"/>
-    <row r="28" spans="11:11"/>
-    <row r="29" spans="11:11"/>
-    <row r="30" spans="11:11"/>
-    <row r="31" spans="11:11"/>
-    <row r="32" spans="11:11"/>
-    <row r="33" spans="11:11"/>
-    <row r="34" spans="11:11"/>
-    <row r="35" spans="11:11"/>
-    <row r="36" spans="11:11"/>
-    <row r="37" spans="11:11"/>
-    <row r="38" spans="11:11"/>
-    <row r="39" spans="11:11"/>
-    <row r="40" spans="11:11"/>
-    <row r="41" spans="11:11"/>
-    <row r="42" spans="11:11"/>
-    <row r="43" spans="11:11"/>
-    <row r="44" spans="11:11"/>
-    <row r="45" spans="11:11"/>
-    <row r="46" spans="11:11"/>
-    <row r="47" spans="11:11"/>
-    <row r="48" spans="11:11"/>
-    <row r="49" spans="11:11"/>
-    <row r="50" spans="11:11"/>
-    <row r="51" spans="11:11"/>
-    <row r="52" spans="11:11"/>
-    <row r="53" spans="11:11"/>
-    <row r="54" spans="11:11"/>
-    <row r="55" spans="11:11"/>
-    <row r="56" spans="11:11"/>
-    <row r="57" spans="11:11"/>
-    <row r="58" spans="11:11"/>
-    <row r="59" spans="11:11"/>
-    <row r="60" spans="11:11"/>
-    <row r="61" spans="11:11"/>
-    <row r="62" spans="11:11"/>
-    <row r="63" spans="11:11"/>
-    <row r="64" spans="11:11"/>
-    <row r="65" spans="11:11"/>
-    <row r="66" spans="11:11"/>
-    <row r="67" spans="11:11"/>
-    <row r="68" spans="11:11"/>
-    <row r="69" spans="11:11"/>
-    <row r="70" spans="11:11"/>
-    <row r="71" spans="11:11"/>
+    <row r="2" spans="10:18">
+      <c r="J2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" s="1"/>
+    </row>
+    <row r="3" spans="10:18"/>
+    <row r="4" spans="10:18"/>
+    <row r="5" spans="10:18"/>
+    <row r="6" spans="10:18"/>
+    <row r="7" spans="10:18"/>
+    <row r="8" spans="10:18"/>
+    <row r="9" spans="10:18"/>
+    <row r="10" spans="10:18"/>
+    <row r="11" spans="10:18"/>
   </sheetData>
   <pageMargins left="1" right="0" top="0.25" bottom="0" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="70" orientation="portrait"/>

</xml_diff>